<commit_message>
form + link edits
</commit_message>
<xml_diff>
--- a/MoSCoW.xlsx
+++ b/MoSCoW.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cameron\Google Drive\UWE\UWE Year 1\Web Design Studio\Semester 2\Portfolio projects\Project 3 - Group website\Project-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1791D966-1D6C-4046-8B0A-00A5999CF6EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C414EB7-34E6-4197-B102-F507254BCE3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,28 +25,67 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Requirement</t>
-  </si>
-  <si>
-    <t>Must have</t>
-  </si>
-  <si>
-    <t>Should have</t>
-  </si>
-  <si>
-    <t>Could have</t>
-  </si>
-  <si>
-    <t>Won't have</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <t>Explorers Southwest</t>
+  </si>
+  <si>
+    <t>Web Design Project 3</t>
+  </si>
+  <si>
+    <t>Must Have</t>
+  </si>
+  <si>
+    <t>Should Have</t>
+  </si>
+  <si>
+    <t>Could Have</t>
+  </si>
+  <si>
+    <t>Won't Have</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Working navigation between </t>
+  </si>
+  <si>
+    <t>pages</t>
+  </si>
+  <si>
+    <t>Multiple pages</t>
+  </si>
+  <si>
+    <t>Gallery</t>
+  </si>
+  <si>
+    <t>Lightboxes</t>
+  </si>
+  <si>
+    <t>Images</t>
+  </si>
+  <si>
+    <t>Contact information</t>
+  </si>
+  <si>
+    <t>A validated form</t>
+  </si>
+  <si>
+    <t>Server side scripting</t>
+  </si>
+  <si>
+    <t>Different methods of navigation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">More than one form </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fluent informative copy to expand business, promote new guided tours to Mesa Verde and attract clients from other states. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -55,6 +94,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -62,45 +110,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -130,59 +148,16 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -194,73 +169,55 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right/>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="5" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="5" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="5" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="2" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="40% - Accent2" xfId="2" builtinId="35"/>
-    <cellStyle name="40% - Accent4" xfId="3" builtinId="43"/>
-    <cellStyle name="40% - Accent5" xfId="4" builtinId="47"/>
-    <cellStyle name="40% - Accent6" xfId="5" builtinId="51"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -274,6 +231,72 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>47699</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="What is MoSCoW Prioritization? | Overview of the MoSCoW Method">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBB7B82F-90C6-4F91-98BE-6D8A7151A413}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="619125" y="771525"/>
+          <a:ext cx="5895975" cy="3086174"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -539,54 +562,133 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:F3"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="22" style="4" customWidth="1"/>
-    <col min="5" max="5" width="21.5703125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="88.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="17"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="21"/>
-    </row>
-    <row r="2" spans="2:6" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="12" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="14" t="s">
+    </row>
+    <row r="5" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="8"/>
+      <c r="D5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="F5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="H5" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="11"/>
+      <c r="J5" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J8" s="11"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="11"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F12" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D13" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="11"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D15" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="11"/>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="11"/>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="11"/>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="11"/>
+    </row>
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D24" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="D17:D21"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changes to MoSCoW file and references
</commit_message>
<xml_diff>
--- a/MoSCoW.xlsx
+++ b/MoSCoW.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cameron\Google Drive\UWE\UWE Year 1\Web Design Studio\Semester 2\Portfolio projects\Project 3 - Group website\Project-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C414EB7-34E6-4197-B102-F507254BCE3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61DF051F-FFF8-45A0-8F33-CC4FF2EB5E23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Explorers Southwest</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t xml:space="preserve">Fluent informative copy to expand business, promote new guided tours to Mesa Verde and attract clients from other states. </t>
+  </si>
+  <si>
+    <t>Location information</t>
   </si>
 </sst>
 </file>
@@ -562,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,6 +683,11 @@
         <v>13</v>
       </c>
     </row>
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D26" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="J7:J8"/>

</xml_diff>

<commit_message>
documentation update with iterations and moscow
</commit_message>
<xml_diff>
--- a/MoSCoW.xlsx
+++ b/MoSCoW.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cameron\Google Drive\UWE\UWE Year 1\Web Design Studio\Semester 2\Portfolio projects\Project 3 - Group website\Project-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61DF051F-FFF8-45A0-8F33-CC4FF2EB5E23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9D6801-C471-47A2-92A7-F7F2C2D5FB01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -242,13 +242,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>47699</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -565,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A3:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,96 +581,90 @@
     <col min="10" max="10" width="11.140625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="J1" s="5"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="D3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="J3" s="5"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
-      <c r="D5" s="10" t="s">
+    <row r="7" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="D7" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F7" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="J7" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D7" s="6" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="11" t="s">
+      <c r="J9" s="11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J8" s="11"/>
-    </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D10" s="6" t="s">
+      <c r="J10" s="11"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D12" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H12" s="11" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D11" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H11" s="11"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F12" s="11" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D13" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="11"/>
+        <v>7</v>
+      </c>
+      <c r="H13" s="11"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F14" s="11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="11"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="4:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D17" s="11" t="s">
+    <row r="19" spans="4:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="11" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D18" s="11"/>
-    </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D19" s="11"/>
     </row>
     <row r="20" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D20" s="11"/>
@@ -678,22 +672,28 @@
     <row r="21" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D21" s="11"/>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D24" s="6" t="s">
-        <v>13</v>
-      </c>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D22" s="11"/>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D23" s="11"/>
     </row>
     <row r="26" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D26" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="6" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="D17:D21"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="D19:D23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>